<commit_message>
Update the definition of Channel ID
</commit_message>
<xml_diff>
--- a/antibodies/latest/antibodies.xlsx
+++ b/antibodies/latest/antibodies.xlsx
@@ -22,7 +22,10 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Structure of the identifier depends on the assay type.</t>
+        <t>(Required) Structure of the identifier depends on the acquisition system.
+Whenever possible this should exactly match the channel ID in the OME TIFF file.
+For example the channel ID in an OME TIFF might be something like "Channel:0:13"
+which would then be the value entered here.</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
@@ -152,7 +155,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-12-11T13:51:31-08:00</t>
+    <t>2024-11-05T13:43:22-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -243,17 +246,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="10.55859375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="3" width="12.73046875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="4" width="12.90234375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="5" width="24.88671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="11.21484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="13.98046875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="8" width="27.515625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="9" width="26.35546875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="10" width="22.34375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="11" width="14.71875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="12" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="9.109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="10.984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="4" width="11.12890625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="5" width="21.46875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="9.67578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="7" width="12.05859375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="8" width="23.734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="9" width="22.734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="10" width="19.2734375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="11" width="12.6953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="12" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -292,7 +295,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="12">
         <v>13</v>
       </c>
     </row>
@@ -325,10 +328,10 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -345,37 +348,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="79.58203125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.20703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="68.6484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Set lot_number as optional
Closes #78
</commit_message>
<xml_diff>
--- a/antibodies/latest/antibodies.xlsx
+++ b/antibodies/latest/antibodies.xlsx
@@ -49,8 +49,8 @@
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) The lot number is specific to the vendor. Example: Abcam lot number
-is GR3238979-1</t>
+        <t>The lot number is specific to the vendor. Example: Abcam lot number is
+GR3238979-1</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
@@ -155,7 +155,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-11-05T13:43:22-08:00</t>
+    <t>2025-03-14T19:47:05-04:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>

</xml_diff>